<commit_message>
added some swtiching functionality
</commit_message>
<xml_diff>
--- a/UI objects.xlsx
+++ b/UI objects.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alden\Documents\Shiny\Data Explorer\Dev\V2-00a\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alden\Documents\Shiny\GitHub\Data-Explorer\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$H$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$F$63</definedName>
   </definedNames>
   <calcPr calcId="171027"/>
   <fileRecoveryPr autoRecover="0"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="116">
   <si>
     <t>Name</t>
   </si>
@@ -111,9 +111,6 @@
     <t>selectInput (multiple)</t>
   </si>
   <si>
-    <t>renderUI</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -219,9 +216,6 @@
     <t>axes to standardize</t>
   </si>
   <si>
-    <t>models to fit</t>
-  </si>
-  <si>
     <t>x axis label</t>
   </si>
   <si>
@@ -312,9 +306,6 @@
     <t>Spacing.Group</t>
   </si>
   <si>
-    <t>shinyjs action</t>
-  </si>
-  <si>
     <t>sliderInput</t>
   </si>
   <si>
@@ -373,6 +364,18 @@
   </si>
   <si>
     <t>thickness of the linear fit(s</t>
+  </si>
+  <si>
+    <t>Testing</t>
+  </si>
+  <si>
+    <t>NOT FUNCTIONAL AND HIDDEN - CAN GO</t>
+  </si>
+  <si>
+    <t>Models</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -401,7 +404,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -411,6 +414,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,7 +445,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -444,6 +453,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,11 +769,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDE2E5A0-CB88-404F-91E5-F0F45A14C774}">
-  <dimension ref="A1:H64"/>
+  <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A40" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B58" sqref="B58"/>
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -772,13 +783,13 @@
     <col min="3" max="3" width="17.73046875" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.53125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.06640625" style="2"/>
+    <col min="6" max="16384" width="9.06640625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="3"/>
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="4" t="s">
+        <v>115</v>
+      </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
@@ -786,246 +797,237 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A2" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A2" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" s="4" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>27</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="4" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A13" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H14" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" s="4" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+        <v>27</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="4" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A15" s="3"/>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A16" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
       <c r="B17" s="2" t="s">
         <v>7</v>
@@ -1034,13 +1036,13 @@
         <v>22</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>3</v>
       </c>
@@ -1048,41 +1050,35 @@
         <v>22</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H18" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
         <v>2</v>
       </c>
@@ -1090,46 +1086,46 @@
         <v>22</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H21" s="2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B22" s="2" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
         <v>5</v>
       </c>
@@ -1137,13 +1133,13 @@
         <v>24</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.45">
+        <v>27</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
@@ -1151,431 +1147,406 @@
         <v>24</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A27" s="7"/>
+      <c r="B27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B28" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" s="4" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A30" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F30" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B27" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" s="4" customFormat="1" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A28" s="3"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A29" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B30" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B32" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F31" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H31" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B32" s="2" t="s">
-        <v>98</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F32" s="2" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
-        <v>105</v>
+        <v>95</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
-        <v>10</v>
+        <v>102</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F34" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
-        <v>96</v>
+        <v>11</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>95</v>
+        <v>25</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.45">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B38" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="F37" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B38" s="2" t="s">
-        <v>16</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>25</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H38" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B39" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H39" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F39" s="2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B40" s="2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C40" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="H40" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A41" s="2"/>
+      <c r="F40" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B41" s="2" t="s">
-        <v>77</v>
+        <v>20</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>78</v>
+        <v>25</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A42" s="2"/>
       <c r="B42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B43" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B43" s="2" t="s">
-        <v>9</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H43" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F43" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B44" s="2" t="s">
-        <v>97</v>
+        <v>9</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.45">
+      <c r="F44" s="2" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B45" s="2" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F45" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B46" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B47" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="C46" s="2" t="s">
+      <c r="C47" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H46" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B47" s="2" t="s">
+      <c r="F47" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B48" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F47" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B48" s="2" t="s">
+      <c r="C48" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B49" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C48" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B49" s="2" t="s">
-        <v>109</v>
-      </c>
       <c r="C49" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.45">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B50" s="2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B51" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B52" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C52" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C51" s="2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B52" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="C52" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F52" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.45">
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B53" s="2" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.45">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B54" s="2" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B55" s="2" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C55" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B56" s="2" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C56" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
       <c r="B57" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="58" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A58" s="5"/>
-      <c r="B58" s="6" t="s">
-        <v>113</v>
-      </c>
-      <c r="C58" s="6" t="s">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B58" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C58" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H58" s="6" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B59" s="2" t="s">
+    </row>
+    <row r="59" spans="1:6" s="6" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="A59" s="5"/>
+      <c r="B59" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="C59" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F59" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B60" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="B61" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C59" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="H59" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A61" s="1" t="s">
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A63" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B63" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F63" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A64" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B61" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="H61" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="A62" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B62" s="2" t="s">
+      <c r="B64" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="C62" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D62" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E62" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B63" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D63" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E63" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.45">
-      <c r="B64" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="C64" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>44</v>
+        <v>27</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B65" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E65" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.45">
+      <c r="B66" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C66" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F66" s="2" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="B2:H61">
-    <sortCondition descending="1" ref="E4:E61"/>
+  <sortState ref="B2:F63">
+    <sortCondition descending="1" ref="E4:E63"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>